<commit_message>
Started local term checks
</commit_message>
<xml_diff>
--- a/test/example-invalid-data.xlsx
+++ b/test/example-invalid-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\model\niem-model-format-spreadsheet\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2B893D-9562-43CC-8DF5-367D860C3D02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDDD565-92F9-4812-990E-7EEDDA6F9AD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10545" yWindow="1620" windowWidth="19440" windowHeight="11670" tabRatio="890" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10545" yWindow="1620" windowWidth="19440" windowHeight="11670" tabRatio="890" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" r:id="rId1"/>
@@ -9778,7 +9778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -9983,11 +9983,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10033,16 +10033,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0800-000001000000}"/>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>MAPPING_CODES</formula1>
     </dataValidation>
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1" xr:uid="{00000000-0002-0000-0800-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>